<commit_message>
renaming control training script
</commit_message>
<xml_diff>
--- a/microscopic/overview.xlsx
+++ b/microscopic/overview.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://scrippsresearch-my.sharepoint.com/personal/amaes_scripps_edu/Documents/Documents/Diffusion_project/DDPM-mouse-behavior/microscopic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="202" documentId="11_F25DC773A252ABDACC104890011D4B745ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B4AE311-5F20-495A-A094-8B6F04B49AC2}"/>
+  <xr:revisionPtr revIDLastSave="442" documentId="11_F25DC773A252ABDACC104890011D4B745ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E89A1678-6E14-416C-B533-79C8CF5BC843}"/>
   <bookViews>
-    <workbookView xWindow="1365" yWindow="2100" windowWidth="25965" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29145" yWindow="1050" windowWidth="27945" windowHeight="13215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="CODE AND FOLDERS AND MODELS" sheetId="1" r:id="rId1"/>
+    <sheet name="LINKING MICE AND VIDEOS" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="188">
   <si>
     <t>Model name</t>
   </si>
@@ -216,9 +217,6 @@
     <t>training.py</t>
   </si>
   <si>
-    <t>training_ctr.py</t>
-  </si>
-  <si>
     <t>training_testing.py</t>
   </si>
   <si>
@@ -262,6 +260,338 @@
   </si>
   <si>
     <t>feedforward model</t>
+  </si>
+  <si>
+    <t>training_behavioral_cloning.py</t>
+  </si>
+  <si>
+    <t>(need to be inside code directory)</t>
+  </si>
+  <si>
+    <t>BALANCED DATASET</t>
+  </si>
+  <si>
+    <t>PHASE A</t>
+  </si>
+  <si>
+    <t>PHASE B</t>
+  </si>
+  <si>
+    <t>PHASE C</t>
+  </si>
+  <si>
+    <t>43 mice</t>
+  </si>
+  <si>
+    <t>7 mice, the first 36 are cut</t>
+  </si>
+  <si>
+    <t>MOUSE NUMBER</t>
+  </si>
+  <si>
+    <t>SLEAP TRACKING</t>
+  </si>
+  <si>
+    <t>labels.90.00_490a_2022-05-11.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.90.01_492a_2022-05-13.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.90.02_504a_2022-05-17.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.90.03_505a_2022-05-17.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.90.04_521a_2022-06-01.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.90.05_534a_2022-06-07.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.90.06_540a_2022-06-08.analysis.h5</t>
+  </si>
+  <si>
+    <t>Phase 1</t>
+  </si>
+  <si>
+    <t>Phase B</t>
+  </si>
+  <si>
+    <t>Phase C</t>
+  </si>
+  <si>
+    <t>labels.1.00_483b_2022-05-11.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.1.01_491b_2022-05-13.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.1.02_502b_2022-05-18.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.1.03_516b_2022-06-01.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.1.04_530b_2022-06-07.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.1.05_535b_2022-06-08.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.1.06_542b_2022-06-15.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.1.07_562b_2022-06-24.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.3.00_484b_2022-05-11.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.3.01_486b_2022-05-13.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.3.02_501b_2022-05-18.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.3.03_513b_2022-05-27.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.3.04_517b_2022-06-01.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.3.05_531b_2022-06-07.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.3.06_536b_2022-06-08.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.3.07_543b_2022-06-16.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.3.08_559b_2022-06-22.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.3.09_563b_2022-06-24.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.10.00_488b_2022-05-13.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.10.01_489b_2022-05-11.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.10.02_503b_2022-05-17.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.10.03_514b_2022-05-27.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.10.04_518b_2022-06-01.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.10.05_537b_2022-06-08.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.10.06_544b_2022-06-15.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.10.07_560b_2022-06-22.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.10.08_564b_2022-06-24.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.30.00_485b_2022-05-11.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.30.01_487b_2022-05-13.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.30.02_500b_2022-05-17.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.30.03_515b_2022-05-27.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.30.04_520b_2022-06-01.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.30.05_533b_2022-06-07.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.30.06_538b_2022-06-08.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.30.07_561b_2022-06-22.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.30.08_565b_2022-06-24.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.90.00_490b_2022-05-11.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.90.01_492b_2022-05-13.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.90.02_504b_2022-05-17.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.90.03_505b_2022-05-17.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.90.04_521b_2022-06-01.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.90.05_534b_2022-06-07.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.90.06_540b_2022-06-08.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.1.00_483c_2022-05-11.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.1.01_491c_2022-05-13.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.1.02_502c_2022-05-18.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.1.03_516c_2022-06-01.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.1.04_530c_2022-06-07.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.1.05_535c_2022-06-08.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.1.06_542c_2022-06-15.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.1.07_562c_2022-06-24.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.3.00_484c_2022-05-11.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.3.01_486c_2022-05-13.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.3.02_501c_2022-05-18.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.3.03_513c_2022-05-27.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.3.04_517c_2022-06-01.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.3.05_531c_2022-06-07.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.3.06_536c_2022-06-08.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.3.07_543c_2022-06-16.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.3.08_559c_2022-06-22.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.3.09_563c_2022-06-24.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.10.00_488c_2022-05-13.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.10.01_489c_2022-05-11.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.10.02_503c_2022-05-17.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.10.03_514c_2022-05-27.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.10.04_518c_2022-06-01.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.10.05_537c_2022-06-08.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.10.06_544c_2022-06-15.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.10.07_560c_2022-06-22.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.10.08_564c_2022-06-24.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.30.00_485c_2022-05-11.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.30.01_487c_2022-05-13.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.30.02_500c_2022-05-17.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.30.03_515c_2022-05-27.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.30.04_520c_2022-06-01.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.30.05_533c_2022-06-07.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.30.06_538c_2022-06-08.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.30.07_561c_2022-06-22.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.30.08_565c_2022-06-24.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.90.00_490c_2022-05-11.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.90.01_492c_2022-05-13.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.90.02_504c_2022-05-17.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.90.03_505c_2022-05-17.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.90.04_521c_2022-06-01.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.90.05_534c_2022-06-07.analysis.h5</t>
+  </si>
+  <si>
+    <t>labels.90.06_540c_2022-06-08.analysis.h5</t>
+  </si>
+  <si>
+    <t>2 hours per model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DURATION SIMULATION </t>
+  </si>
+  <si>
+    <t>2 hours for 93 mice
+(12 in parallel)</t>
+  </si>
+  <si>
+    <t>2 hours for 500 samples
+(12 in parallel)</t>
   </si>
 </sst>
 </file>
@@ -305,10 +635,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,21 +926,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" customWidth="1"/>
     <col min="3" max="3" width="30.5703125" customWidth="1"/>
     <col min="4" max="4" width="28.7109375" customWidth="1"/>
     <col min="5" max="5" width="26.28515625" customWidth="1"/>
     <col min="6" max="6" width="30.7109375" customWidth="1"/>
-    <col min="7" max="7" width="28" customWidth="1"/>
+    <col min="7" max="7" width="28.85546875" customWidth="1"/>
     <col min="8" max="8" width="25" customWidth="1"/>
     <col min="9" max="9" width="22.140625" customWidth="1"/>
   </cols>
@@ -616,7 +949,9 @@
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
@@ -719,29 +1054,29 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>20</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>6</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -889,7 +1224,7 @@
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
@@ -910,127 +1245,955 @@
         <v>14</v>
       </c>
       <c r="I15" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E16" t="s">
+        <v>184</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" s="1" t="s">
+      <c r="C21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H21" s="1" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B21" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" t="s">
-        <v>67</v>
-      </c>
-      <c r="D21" t="s">
-        <v>70</v>
-      </c>
-      <c r="E21" t="s">
-        <v>72</v>
-      </c>
-      <c r="F21" t="s">
-        <v>74</v>
-      </c>
-      <c r="G21" t="s">
-        <v>62</v>
-      </c>
-      <c r="H21" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" t="s">
         <v>71</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>73</v>
       </c>
-      <c r="F22" t="s">
-        <v>75</v>
-      </c>
       <c r="G22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" t="s">
+        <v>74</v>
+      </c>
+      <c r="G23" t="s">
+        <v>78</v>
+      </c>
+      <c r="H23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C23" t="s">
-        <v>69</v>
-      </c>
-      <c r="E23" t="s">
-        <v>76</v>
-      </c>
-      <c r="G23" t="s">
+      <c r="C24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" t="s">
+        <v>75</v>
+      </c>
+      <c r="G24" t="s">
+        <v>63</v>
+      </c>
+      <c r="H24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G25" t="s">
         <v>64</v>
       </c>
-      <c r="H23" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G24" t="s">
-        <v>65</v>
-      </c>
-      <c r="H24" t="s">
+      <c r="H25" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DCC2C02-2060-4DF6-8894-E1D5D124664B}">
+  <dimension ref="A1:B99"/>
+  <sheetViews>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="F99" sqref="F99"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="40.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>16</v>
+      </c>
+      <c r="B21" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>18</v>
+      </c>
+      <c r="B23" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>19</v>
+      </c>
+      <c r="B24" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>20</v>
+      </c>
+      <c r="B25" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>21</v>
+      </c>
+      <c r="B26" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>22</v>
+      </c>
+      <c r="B27" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>23</v>
+      </c>
+      <c r="B28" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>24</v>
+      </c>
+      <c r="B29" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>25</v>
+      </c>
+      <c r="B30" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>26</v>
+      </c>
+      <c r="B31" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>27</v>
+      </c>
+      <c r="B32" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>28</v>
+      </c>
+      <c r="B33" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>29</v>
+      </c>
+      <c r="B34" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>30</v>
+      </c>
+      <c r="B35" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>31</v>
+      </c>
+      <c r="B36" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>32</v>
+      </c>
+      <c r="B37" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>33</v>
+      </c>
+      <c r="B38" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>34</v>
+      </c>
+      <c r="B39" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>35</v>
+      </c>
+      <c r="B40" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>36</v>
+      </c>
+      <c r="B41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>37</v>
+      </c>
+      <c r="B42" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>38</v>
+      </c>
+      <c r="B43" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>39</v>
+      </c>
+      <c r="B44" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>40</v>
+      </c>
+      <c r="B45" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>41</v>
+      </c>
+      <c r="B46" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>42</v>
+      </c>
+      <c r="B47" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>43</v>
+      </c>
+      <c r="B48" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>44</v>
+      </c>
+      <c r="B49" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>45</v>
+      </c>
+      <c r="B50" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>46</v>
+      </c>
+      <c r="B51" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>47</v>
+      </c>
+      <c r="B52" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>48</v>
+      </c>
+      <c r="B53" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>49</v>
+      </c>
+      <c r="B54" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>50</v>
+      </c>
+      <c r="B57" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>51</v>
+      </c>
+      <c r="B58" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>52</v>
+      </c>
+      <c r="B59" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>53</v>
+      </c>
+      <c r="B60" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>54</v>
+      </c>
+      <c r="B61" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>55</v>
+      </c>
+      <c r="B62" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>56</v>
+      </c>
+      <c r="B63" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>57</v>
+      </c>
+      <c r="B64" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>58</v>
+      </c>
+      <c r="B65" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>59</v>
+      </c>
+      <c r="B66" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>60</v>
+      </c>
+      <c r="B67" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>61</v>
+      </c>
+      <c r="B68" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>62</v>
+      </c>
+      <c r="B69" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>63</v>
+      </c>
+      <c r="B70" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>64</v>
+      </c>
+      <c r="B71" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>65</v>
+      </c>
+      <c r="B72" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>66</v>
+      </c>
+      <c r="B73" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>67</v>
+      </c>
+      <c r="B74" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>68</v>
+      </c>
+      <c r="B75" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>69</v>
+      </c>
+      <c r="B76" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>70</v>
+      </c>
+      <c r="B77" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>71</v>
+      </c>
+      <c r="B78" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>72</v>
+      </c>
+      <c r="B79" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>73</v>
+      </c>
+      <c r="B80" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>74</v>
+      </c>
+      <c r="B81" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>75</v>
+      </c>
+      <c r="B82" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>76</v>
+      </c>
+      <c r="B83" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>77</v>
+      </c>
+      <c r="B84" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>78</v>
+      </c>
+      <c r="B85" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>79</v>
+      </c>
+      <c r="B86" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>80</v>
+      </c>
+      <c r="B87" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>81</v>
+      </c>
+      <c r="B88" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>82</v>
+      </c>
+      <c r="B89" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>83</v>
+      </c>
+      <c r="B90" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>84</v>
+      </c>
+      <c r="B91" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>85</v>
+      </c>
+      <c r="B92" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>86</v>
+      </c>
+      <c r="B93" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>87</v>
+      </c>
+      <c r="B94" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>88</v>
+      </c>
+      <c r="B95" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>89</v>
+      </c>
+      <c r="B96" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>90</v>
+      </c>
+      <c r="B97" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>91</v>
+      </c>
+      <c r="B98" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>92</v>
+      </c>
+      <c r="B99" t="s">
+        <v>183</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>